<commit_message>
Rev 3.1 M52 PCB added
</commit_message>
<xml_diff>
--- a/m52_PnP/Rev3.0B documents/BOM-speeduino compatible PCB for m52 rev3.0B (PCBWay).xlsx
+++ b/m52_PnP/Rev3.0B documents/BOM-speeduino compatible PCB for m52 rev3.0B (PCBWay).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52_PnP\Rev3.0B documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE74124-76B4-47EB-A4BC-8A7FC9F750BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBED31C-D25C-49FF-8E1D-ED510F97DE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13785" yWindow="1680" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,9 +196,6 @@
     <t>TSSOP-20_L6.5-W4.4-P0.65-LS6.4-BL</t>
   </si>
   <si>
-    <t>Arduino Mega F407 PCB 1.3 BOM  (Bill of Materials)</t>
-  </si>
-  <si>
     <t>THT</t>
   </si>
   <si>
@@ -461,9 +458,6 @@
   </si>
   <si>
     <t>Bourns</t>
-  </si>
-  <si>
-    <t>Can be substituted with ohter brand 14D220K varistors too</t>
   </si>
   <si>
     <t>onsemi / Fairchild</t>
@@ -562,18 +556,31 @@
   </si>
   <si>
     <t>1A Fixed 5V Positive electrode 26V TO-220 Voltage Regulators - Linear, Low Drop Out (LDO) Regulators</t>
+  </si>
+  <si>
+    <t>Can be substituted with other brand 14D220K varistors too</t>
+  </si>
+  <si>
+    <t>Speeduino compatible PCB for m52 rev3.0B  (Bill of Materials)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -699,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -708,66 +715,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1122,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1141,25 +1146,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="D2" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="D2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -1195,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="8">
         <v>12</v>
@@ -1204,13 +1209,13 @@
         <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>10</v>
@@ -1222,7 +1227,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="8">
         <v>22</v>
@@ -1230,11 +1235,11 @@
       <c r="D8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>71</v>
+      <c r="E8" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>27</v>
@@ -1249,7 +1254,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="8">
         <v>14</v>
@@ -1257,11 +1262,11 @@
       <c r="D9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>120</v>
+      <c r="E9" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>26</v>
@@ -1269,8 +1274,8 @@
       <c r="H9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>111</v>
+      <c r="I9" s="20" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15">
@@ -1278,7 +1283,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="8">
         <v>15</v>
@@ -1286,11 +1291,11 @@
       <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>72</v>
+      <c r="E10" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>27</v>
@@ -1305,19 +1310,19 @@
         <v>5</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="8">
         <v>14</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="D11" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>27</v>
@@ -1332,7 +1337,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
@@ -1340,11 +1345,11 @@
       <c r="D12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="20" t="s">
-        <v>73</v>
+      <c r="E12" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>27</v>
@@ -1359,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="8">
         <v>2</v>
@@ -1367,11 +1372,11 @@
       <c r="D13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>74</v>
+      <c r="E13" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>27</v>
@@ -1386,7 +1391,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="8">
         <v>11</v>
@@ -1394,11 +1399,11 @@
       <c r="D14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>75</v>
+      <c r="E14" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>27</v>
@@ -1413,22 +1418,22 @@
         <v>9</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="8">
         <v>2</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>76</v>
+        <v>60</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>10</v>
@@ -1440,22 +1445,22 @@
         <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>77</v>
+        <v>61</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>10</v>
@@ -1467,19 +1472,19 @@
         <v>11</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="8">
         <v>4</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>78</v>
+        <v>62</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>25</v>
@@ -1494,7 +1499,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="8">
         <v>14</v>
@@ -1502,11 +1507,11 @@
       <c r="D18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="17" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>25</v>
@@ -1521,7 +1526,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="8">
         <v>5</v>
@@ -1529,11 +1534,11 @@
       <c r="D19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>79</v>
+      <c r="E19" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>25</v>
@@ -1548,7 +1553,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="8">
         <v>4</v>
@@ -1556,11 +1561,11 @@
       <c r="D20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="17" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>25</v>
@@ -1575,19 +1580,19 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="8">
         <v>3</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>80</v>
+        <v>62</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>25</v>
@@ -1602,19 +1607,19 @@
         <v>16</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>136</v>
+        <v>62</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>134</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>25</v>
@@ -1629,7 +1634,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="8">
         <v>2</v>
@@ -1637,14 +1642,14 @@
       <c r="D23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="20" t="s">
-        <v>82</v>
+      <c r="E23" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>10</v>
@@ -1656,22 +1661,22 @@
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="8">
         <v>1</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>83</v>
+        <v>63</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>10</v>
@@ -1683,7 +1688,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="8">
         <v>14</v>
@@ -1691,11 +1696,11 @@
       <c r="D25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="20" t="s">
-        <v>84</v>
+      <c r="E25" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>27</v>
@@ -1710,7 +1715,7 @@
         <v>20</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="8">
         <v>3</v>
@@ -1718,11 +1723,11 @@
       <c r="D26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="20" t="s">
-        <v>85</v>
+      <c r="E26" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>27</v>
@@ -1737,22 +1742,22 @@
         <v>21</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="8">
         <v>1</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>141</v>
+        <v>64</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>10</v>
@@ -1764,7 +1769,7 @@
         <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="8">
         <v>1</v>
@@ -1772,11 +1777,11 @@
       <c r="D28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>87</v>
+      <c r="E28" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>25</v>
@@ -1791,22 +1796,22 @@
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="8">
         <v>1</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>88</v>
+        <v>65</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>10</v>
@@ -1824,16 +1829,16 @@
         <v>1</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>89</v>
+        <v>66</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>10</v>
@@ -1845,22 +1850,22 @@
         <v>25</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="8">
         <v>1</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>145</v>
+        <v>63</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>10</v>
@@ -1872,22 +1877,22 @@
         <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>91</v>
+        <v>67</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>10</v>
@@ -1899,25 +1904,25 @@
         <v>27</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="8">
         <v>1</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="22">
+        <v>31</v>
+      </c>
+      <c r="E33" s="19">
         <v>430451600</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1926,7 +1931,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="8">
         <v>1</v>
@@ -1934,11 +1939,11 @@
       <c r="D34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>28</v>
@@ -1953,7 +1958,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="8">
         <v>6</v>
@@ -1961,14 +1966,14 @@
       <c r="D35" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="20" t="s">
-        <v>92</v>
+      <c r="E35" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>10</v>
@@ -1985,46 +1990,46 @@
       <c r="C36" s="8">
         <v>1</v>
       </c>
-      <c r="D36" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="20" t="s">
+      <c r="D36" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>116</v>
-      </c>
       <c r="G36" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15">
       <c r="A37" s="5">
         <v>31</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="8">
         <v>1</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>93</v>
+        <v>68</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H37" s="16" t="s">
         <v>10</v>
@@ -2036,28 +2041,28 @@
         <v>32</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="8">
         <v>6</v>
       </c>
-      <c r="D38" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>94</v>
+      <c r="D38" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15">
@@ -2073,17 +2078,17 @@
       <c r="D39" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="20" t="s">
-        <v>95</v>
+      <c r="E39" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I39" s="15"/>
     </row>

</xml_diff>